<commit_message>
sentiment analysis integrated with the R data analysis
</commit_message>
<xml_diff>
--- a/Tariff_Impact_Analysis_Complete.xlsx
+++ b/Tariff_Impact_Analysis_Complete.xlsx
@@ -10,7 +10,12 @@
     <sheet name="Volatility_Analysis" sheetId="1" r:id="rId1"/>
     <sheet name="Moving_Average_Changes" sheetId="2" r:id="rId2"/>
     <sheet name="Statistical_Tests" sheetId="3" r:id="rId3"/>
-    <sheet name="Raw_Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Overall_Sentiment_Correlations" sheetId="4" r:id="rId4"/>
+    <sheet name="Event_Window_Analysis" sheetId="5" r:id="rId5"/>
+    <sheet name="Correlation_Significance" sheetId="6" r:id="rId6"/>
+    <sheet name="Daily_Sentiment_Summary" sheetId="7" r:id="rId7"/>
+    <sheet name="Raw_Stock_Data" sheetId="8" r:id="rId8"/>
+    <sheet name="Correlation_Summary" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -743,6 +748,771 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>correlation_sentiment</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>correlation_vader</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>n_observations</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CNPF</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>-0.7609799016613027</v>
+      </c>
+      <c r="C2">
+        <v>-0.615471969883548</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GSMI</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>-0.4027456393398635</v>
+      </c>
+      <c r="C3">
+        <v>-0.2822413021159349</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>JFC</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>-0.4171755257640853</v>
+      </c>
+      <c r="C4">
+        <v>-0.2097548491947978</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MONDE</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>-0.2487815445421259</v>
+      </c>
+      <c r="C5">
+        <v>-0.1395955539677381</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>-0.5001911056759699</v>
+      </c>
+      <c r="C6">
+        <v>-0.5322607846706537</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="20.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>correlation</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>avg_return</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>avg_sentiment</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>n_obs</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>event_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CNPF</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>-4.341736694677882</v>
+      </c>
+      <c r="D2">
+        <v>0.2775</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GSMI</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>-1.947623261719669</v>
+      </c>
+      <c r="D3">
+        <v>0.2775</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>JFC</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>-3.114186851211068</v>
+      </c>
+      <c r="D4">
+        <v>0.2775</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MONDE</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>-2.906208718626164</v>
+      </c>
+      <c r="D5">
+        <v>0.2775</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>-1.140413399857465</v>
+      </c>
+      <c r="D6">
+        <v>0.2775</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CNPF</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>-0.796052911302524</v>
+      </c>
+      <c r="C7">
+        <v>-0.8175510518010118</v>
+      </c>
+      <c r="D7">
+        <v>-0.009466666666666665</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45848</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GSMI</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>0.9711599613451505</v>
+      </c>
+      <c r="C8">
+        <v>0.06910850034554512</v>
+      </c>
+      <c r="D8">
+        <v>-0.009466666666666665</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45848</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>JFC</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>-0.6907008212888047</v>
+      </c>
+      <c r="C9">
+        <v>-0.1449163598580867</v>
+      </c>
+      <c r="D9">
+        <v>-0.009466666666666665</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>45848</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MONDE</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>0.9951280168714758</v>
+      </c>
+      <c r="C10">
+        <v>2.000255770647278</v>
+      </c>
+      <c r="D10">
+        <v>-0.009466666666666665</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2">
+        <v>45848</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>-0.6298166871152562</v>
+      </c>
+      <c r="C11">
+        <v>0.3675537253512813</v>
+      </c>
+      <c r="D11">
+        <v>-0.009466666666666665</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>45848</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>correlation</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>p_value</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>significant</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>n_observations</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>JFC</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>-0.4171755257640853</v>
+      </c>
+      <c r="C2">
+        <v>0.2639428999346807</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>-0.5001911056759699</v>
+      </c>
+      <c r="C3">
+        <v>0.1702810694466928</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CNPF</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>-0.7609799016613027</v>
+      </c>
+      <c r="C4">
+        <v>0.01724163872013969</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GSMI</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>-0.4027456393398635</v>
+      </c>
+      <c r="C5">
+        <v>0.2824997426247369</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MONDE</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>-0.2487815445421259</v>
+      </c>
+      <c r="C6">
+        <v>0.5186036260194442</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>avg_sentiment</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>sentiment_count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>avg_vader</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>45631</v>
+      </c>
+      <c r="B2">
+        <v>-0.4398</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>-0.9883</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>45702</v>
+      </c>
+      <c r="B3">
+        <v>-0.4232</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>-0.9136</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>45743</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>45750</v>
+      </c>
+      <c r="B5">
+        <v>0.2775</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0.3488</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>45753</v>
+      </c>
+      <c r="B6">
+        <v>0.0682</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>45794</v>
+      </c>
+      <c r="B7">
+        <v>-0.583</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>-0.7909</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>45806</v>
+      </c>
+      <c r="B8">
+        <v>-0.3877</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>-0.842</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>45829</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>45836</v>
+      </c>
+      <c r="B10">
+        <v>-0.2772</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>-0.2732</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>45845</v>
+      </c>
+      <c r="B11">
+        <v>-0.1132</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>-0.2263</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>45848</v>
+      </c>
+      <c r="B12">
+        <v>0.1361</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>0.2229428571428571</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <v>45849</v>
+      </c>
+      <c r="B13">
+        <v>-0.0513</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>-0.1027</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <v>45850</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <v>45856</v>
+      </c>
+      <c r="B15">
+        <v>-0.25</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2">
+        <v>45861</v>
+      </c>
+      <c r="B16">
+        <v>0.07028571428571428</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>0.174</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <v>45862</v>
+      </c>
+      <c r="B17">
+        <v>0.541</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0.9712</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AO137"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17427,4 +18197,89 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Companies with |r| &gt; 0.3</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Significant correlations (p &lt; 0.05)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Average correlation</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>-0.466</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sentiment data points</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Date range</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-02-14 to 2025-07-23</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed the tariff dates.
</commit_message>
<xml_diff>
--- a/Tariff_Impact_Analysis_Complete.xlsx
+++ b/Tariff_Impact_Analysis_Complete.xlsx
@@ -920,7 +920,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>45750</v>
+        <v>45749</v>
       </c>
     </row>
     <row r="3">
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>45750</v>
+        <v>45749</v>
       </c>
     </row>
     <row r="4">
@@ -958,7 +958,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>45750</v>
+        <v>45749</v>
       </c>
     </row>
     <row r="5">
@@ -977,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2">
-        <v>45750</v>
+        <v>45749</v>
       </c>
     </row>
     <row r="6">
@@ -996,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2">
-        <v>45750</v>
+        <v>45749</v>
       </c>
     </row>
     <row r="7">
@@ -1018,7 +1018,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="2">
-        <v>45848</v>
+        <v>45847</v>
       </c>
     </row>
     <row r="8">
@@ -1040,7 +1040,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="2">
-        <v>45848</v>
+        <v>45847</v>
       </c>
     </row>
     <row r="9">
@@ -1062,7 +1062,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="2">
-        <v>45848</v>
+        <v>45847</v>
       </c>
     </row>
     <row r="10">
@@ -1084,7 +1084,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="2">
-        <v>45848</v>
+        <v>45847</v>
       </c>
     </row>
     <row r="11">
@@ -1106,7 +1106,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="2">
-        <v>45848</v>
+        <v>45847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>